<commit_message>
Fixed output of Ladder columns
</commit_message>
<xml_diff>
--- a/Normalization.xlsx
+++ b/Normalization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HenriLACHAIZE\PycharmProjects\Normalization_Pump_OT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B5F659-ED2A-454E-8BE8-9F79E730A8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C56751-B45E-4801-A2BA-0EFB7C03F4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -986,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4150,18 +4150,12 @@
       <c r="A76" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="41">
-        <v>24</v>
-      </c>
+      <c r="B76" s="41"/>
       <c r="C76" s="41">
         <v>24</v>
       </c>
-      <c r="D76" s="41">
-        <v>30</v>
-      </c>
-      <c r="E76" s="41">
-        <v>50</v>
-      </c>
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
       <c r="F76" s="41">
         <v>24</v>
       </c>
@@ -4174,18 +4168,10 @@
       <c r="I76" s="41">
         <v>50</v>
       </c>
-      <c r="J76" s="41">
-        <v>20</v>
-      </c>
-      <c r="K76" s="41">
-        <v>50</v>
-      </c>
-      <c r="L76" s="41">
-        <v>25</v>
-      </c>
-      <c r="M76" s="41">
-        <v>25</v>
-      </c>
+      <c r="J76" s="41"/>
+      <c r="K76" s="41"/>
+      <c r="L76" s="41"/>
+      <c r="M76" s="41"/>
       <c r="Q76" s="47" t="s">
         <v>4</v>
       </c>
@@ -4232,7 +4218,7 @@
       </c>
       <c r="B77" s="50">
         <f>B$76</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C77" s="50">
         <f t="shared" ref="C77:M77" si="8">C$76</f>
@@ -4240,11 +4226,11 @@
       </c>
       <c r="D77" s="50">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E77" s="50">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F77" s="50">
         <f t="shared" si="8"/>
@@ -4264,19 +4250,19 @@
       </c>
       <c r="J77" s="50">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K77" s="50">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L77" s="50">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M77" s="50">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q77" s="47" t="s">
         <v>5</v>
@@ -4336,51 +4322,51 @@
       </c>
       <c r="B78" s="50">
         <f t="shared" ref="B78:M83" si="10">B$76</f>
+        <v>0</v>
+      </c>
+      <c r="C78" s="50">
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="C78" s="50">
+      <c r="D78" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F78" s="50">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="D78" s="50">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="E78" s="50">
+      <c r="G78" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="H78" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="I78" s="50">
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="F78" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="G78" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="H78" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="I78" s="50">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
       <c r="J78" s="50">
         <f t="shared" si="10"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K78" s="50">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L78" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M78" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P78" s="3"/>
       <c r="Q78" s="47" t="s">
@@ -4441,51 +4427,51 @@
       </c>
       <c r="B79" s="50">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C79" s="50">
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="C79" s="50">
+      <c r="D79" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E79" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="50">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="D79" s="50">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="E79" s="50">
+      <c r="G79" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="H79" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="I79" s="50">
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="F79" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="G79" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="H79" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="I79" s="50">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
       <c r="J79" s="50">
         <f t="shared" si="10"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K79" s="50">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L79" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M79" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P79" s="3"/>
       <c r="Q79" s="47" t="s">
@@ -4546,51 +4532,51 @@
       </c>
       <c r="B80" s="50">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C80" s="50">
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="C80" s="50">
+      <c r="D80" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E80" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F80" s="50">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="D80" s="50">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="E80" s="50">
+      <c r="G80" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="H80" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="I80" s="50">
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="F80" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="G80" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="H80" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="I80" s="50">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
       <c r="J80" s="50">
         <f t="shared" si="10"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K80" s="50">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L80" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M80" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P80" s="4"/>
       <c r="Q80" s="47" t="s">
@@ -4651,51 +4637,51 @@
       </c>
       <c r="B81" s="50">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C81" s="50">
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="C81" s="50">
+      <c r="D81" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E81" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F81" s="50">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="D81" s="50">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="E81" s="50">
+      <c r="G81" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="H81" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="I81" s="50">
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="F81" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="G81" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="H81" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="I81" s="50">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
       <c r="J81" s="50">
         <f t="shared" si="10"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K81" s="50">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L81" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M81" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q81" s="47" t="s">
         <v>9</v>
@@ -4755,51 +4741,51 @@
       </c>
       <c r="B82" s="50">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C82" s="50">
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="C82" s="50">
+      <c r="D82" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E82" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F82" s="50">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="D82" s="50">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="E82" s="50">
+      <c r="G82" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="H82" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="I82" s="50">
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="F82" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="G82" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="H82" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="I82" s="50">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
       <c r="J82" s="50">
         <f t="shared" si="10"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K82" s="50">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L82" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M82" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q82" s="47" t="s">
         <v>10</v>
@@ -4859,51 +4845,51 @@
       </c>
       <c r="B83" s="50">
         <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="C83" s="50">
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="C83" s="50">
+      <c r="D83" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="50">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="50">
         <f t="shared" si="10"/>
         <v>24</v>
       </c>
-      <c r="D83" s="50">
-        <f t="shared" si="10"/>
-        <v>30</v>
-      </c>
-      <c r="E83" s="50">
+      <c r="G83" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="H83" s="50">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="I83" s="50">
         <f t="shared" si="10"/>
         <v>50</v>
       </c>
-      <c r="F83" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="G83" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="H83" s="50">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="I83" s="50">
-        <f t="shared" si="10"/>
-        <v>50</v>
-      </c>
       <c r="J83" s="50">
         <f t="shared" si="10"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K83" s="50">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="L83" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M83" s="50">
         <f t="shared" si="10"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q83" s="47" t="s">
         <v>11</v>

</xml_diff>